<commit_message>
Create individual .sas files for code
Split SAS project (.egp) into separate .sas programs for ease of grading
</commit_message>
<xml_diff>
--- a/Assignment 1/Table_4.xlsx
+++ b/Assignment 1/Table_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phoebelu/Documents/UCLA/WQ2022/EPI207/EPIDEM207-2022-winter/Assignment 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFE4619-A655-874C-A93D-36C9C07719DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C2969B-6E35-CB49-8B04-B93D6353BE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17740" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -338,18 +338,6 @@
     <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -365,6 +353,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -374,10 +368,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -525,27 +525,35 @@
     <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="3" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
+      <c r="A3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
@@ -557,10 +565,10 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
@@ -584,143 +592,143 @@
       <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="7"/>
+      <c r="I5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16" t="s">
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
     </row>
     <row r="6" spans="1:16" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="H6" s="11"/>
-      <c r="I6" s="12" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="13" t="s">
+      <c r="K6" s="16"/>
+      <c r="L6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="13" t="s">
+      <c r="O6" s="16"/>
+      <c r="P6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="H7" s="11" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="H7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="10">
         <v>5.92</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="11">
         <v>4.9740000000000002</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="11">
         <v>7.0449999999999999</v>
       </c>
-      <c r="L7" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" s="15">
+      <c r="L7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="11">
         <v>10.452999999999999</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="11">
         <v>7.258</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="11">
         <v>15.054</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="P7" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="12">
         <v>5.0709999999999997</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="12">
         <v>4.22</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="12">
         <v>6.0940000000000003</v>
       </c>
-      <c r="L8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" s="19">
+      <c r="L8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="12">
         <v>10.276</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="12">
         <v>6.9139999999999997</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="12">
         <v>15.271000000000001</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="P8" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="H9" s="11" t="s">
+      <c r="A9" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="H9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="12">
         <v>2.3759999999999999</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="12">
         <v>1.9610000000000001</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="12">
         <v>2.879</v>
       </c>
-      <c r="L9" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="M9" s="19">
+      <c r="L9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="12">
         <v>3.605</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="12">
         <v>2.4409999999999998</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="12">
         <v>5.3220000000000001</v>
       </c>
-      <c r="P9" s="20" t="s">
+      <c r="P9" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -734,38 +742,38 @@
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="12">
         <v>2.1949999999999998</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="12">
         <v>1.7549999999999999</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="12">
         <v>2.7440000000000002</v>
       </c>
-      <c r="L10" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" s="19">
+      <c r="L10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="12">
         <v>3.2429999999999999</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="12">
         <v>2.129</v>
       </c>
-      <c r="O10" s="19">
+      <c r="O10" s="12">
         <v>4.9390000000000001</v>
       </c>
-      <c r="P10" s="20" t="s">
+      <c r="P10" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -788,82 +796,82 @@
       <c r="F11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="12">
         <v>2.1819999999999999</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="12">
         <v>1.744</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="12">
         <v>2.73</v>
       </c>
-      <c r="L11" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="M11" s="19">
+      <c r="L11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="12">
         <v>3.17</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="12">
         <v>2.0779999999999998</v>
       </c>
-      <c r="O11" s="19">
+      <c r="O11" s="12">
         <v>4.835</v>
       </c>
-      <c r="P11" s="20" t="s">
+      <c r="P11" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="12">
         <v>2.069</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="12">
         <v>1.65</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="12">
         <v>2.5950000000000002</v>
       </c>
-      <c r="L12" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" s="19">
+      <c r="L12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="12">
         <v>3.0470000000000002</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="12">
         <v>1.992</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O12" s="12">
         <v>4.66</v>
       </c>
-      <c r="P12" s="20" t="s">
+      <c r="P12" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="15" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="A15" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
@@ -875,10 +883,10 @@
       <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="2" t="s">
         <v>6</v>
       </c>
@@ -944,24 +952,24 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="23" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="A23" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
@@ -973,10 +981,10 @@
       <c r="C24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="2" t="s">
         <v>6</v>
       </c>
@@ -1042,24 +1050,24 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
     </row>
     <row r="31" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="A31" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
     </row>
     <row r="32" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
@@ -1071,10 +1079,10 @@
       <c r="C32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="20"/>
       <c r="F32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1160,24 +1168,24 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
     </row>
     <row r="40" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="A40" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
     </row>
     <row r="41" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
@@ -1189,10 +1197,10 @@
       <c r="C41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="7"/>
+      <c r="E41" s="20"/>
       <c r="F41" s="2" t="s">
         <v>6</v>
       </c>
@@ -1278,34 +1286,34 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
     </row>
     <row r="48" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
     </row>
     <row r="50" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
+      <c r="A50" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
     </row>
     <row r="51" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
@@ -1317,10 +1325,10 @@
       <c r="C51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E51" s="7"/>
+      <c r="E51" s="20"/>
       <c r="F51" s="2" t="s">
         <v>6</v>
       </c>
@@ -1466,34 +1474,34 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
     </row>
     <row r="61" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="10" t="s">
+      <c r="A61" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
     </row>
     <row r="63" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
+      <c r="A63" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
     </row>
     <row r="64" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
@@ -1505,10 +1513,10 @@
       <c r="C64" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E64" s="7"/>
+      <c r="E64" s="20"/>
       <c r="F64" s="2" t="s">
         <v>6</v>
       </c>
@@ -1654,34 +1662,34 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
     </row>
     <row r="74" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
     </row>
     <row r="76" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
+      <c r="A76" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="20"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
     </row>
     <row r="77" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
@@ -1693,10 +1701,10 @@
       <c r="C77" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="7"/>
+      <c r="E77" s="20"/>
       <c r="F77" s="2" t="s">
         <v>6</v>
       </c>
@@ -1882,34 +1890,34 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="8" t="s">
+      <c r="A88" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
     </row>
     <row r="89" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="10" t="s">
+      <c r="A89" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B89" s="9"/>
-      <c r="C89" s="9"/>
-      <c r="D89" s="9"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="9"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
     </row>
     <row r="91" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="7"/>
+      <c r="A91" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" s="20"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="20"/>
     </row>
     <row r="92" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
@@ -1921,10 +1929,10 @@
       <c r="C92" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D92" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E92" s="7"/>
+      <c r="E92" s="20"/>
       <c r="F92" s="2" t="s">
         <v>6</v>
       </c>
@@ -2110,34 +2118,34 @@
       </c>
     </row>
     <row r="103" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="8" t="s">
+      <c r="A103" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B103" s="9"/>
-      <c r="C103" s="9"/>
-      <c r="D103" s="9"/>
-      <c r="E103" s="9"/>
-      <c r="F103" s="9"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
     </row>
     <row r="104" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="10" t="s">
+      <c r="A104" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B104" s="9"/>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="9"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
     </row>
     <row r="106" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
-      <c r="F106" s="7"/>
+      <c r="A106" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B106" s="20"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="20"/>
+      <c r="F106" s="20"/>
     </row>
     <row r="107" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
@@ -2149,10 +2157,10 @@
       <c r="C107" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D107" s="7" t="s">
+      <c r="D107" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E107" s="7"/>
+      <c r="E107" s="20"/>
       <c r="F107" s="2" t="s">
         <v>6</v>
       </c>
@@ -2358,34 +2366,34 @@
       </c>
     </row>
     <row r="119" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="8" t="s">
+      <c r="A119" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B119" s="9"/>
-      <c r="C119" s="9"/>
-      <c r="D119" s="9"/>
-      <c r="E119" s="9"/>
-      <c r="F119" s="9"/>
+      <c r="B119" s="18"/>
+      <c r="C119" s="18"/>
+      <c r="D119" s="18"/>
+      <c r="E119" s="18"/>
+      <c r="F119" s="18"/>
     </row>
     <row r="120" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="10" t="s">
+      <c r="A120" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B120" s="9"/>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
+      <c r="B120" s="18"/>
+      <c r="C120" s="18"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="18"/>
+      <c r="F120" s="18"/>
     </row>
     <row r="122" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B122" s="7"/>
-      <c r="C122" s="7"/>
-      <c r="D122" s="7"/>
-      <c r="E122" s="7"/>
-      <c r="F122" s="7"/>
+      <c r="A122" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B122" s="20"/>
+      <c r="C122" s="20"/>
+      <c r="D122" s="20"/>
+      <c r="E122" s="20"/>
+      <c r="F122" s="20"/>
     </row>
     <row r="123" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
@@ -2397,10 +2405,10 @@
       <c r="C123" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D123" s="7" t="s">
+      <c r="D123" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E123" s="7"/>
+      <c r="E123" s="20"/>
       <c r="F123" s="2" t="s">
         <v>6</v>
       </c>
@@ -2607,16 +2615,11 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="A103:F103"/>
-    <mergeCell ref="A104:F104"/>
-    <mergeCell ref="A119:F119"/>
-    <mergeCell ref="A120:F120"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="A106:F106"/>
-    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A15:F15"/>
     <mergeCell ref="A122:F122"/>
     <mergeCell ref="D123:E123"/>
     <mergeCell ref="A1:F1"/>
@@ -2633,6 +2636,11 @@
     <mergeCell ref="A74:F74"/>
     <mergeCell ref="D64:E64"/>
     <mergeCell ref="A76:F76"/>
+    <mergeCell ref="A119:F119"/>
+    <mergeCell ref="A120:F120"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="A106:F106"/>
+    <mergeCell ref="D107:E107"/>
     <mergeCell ref="D77:E77"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="D92:E92"/>
@@ -2644,15 +2652,15 @@
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="A63:F63"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="A103:F103"/>
+    <mergeCell ref="A104:F104"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A15:F15"/>
   </mergeCells>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>